<commit_message>
Fix: Models & Feature: Menambahkan 1 Controller Models: Ubah nama tabel dan beberapa nama kolom di tabel data_diri. Menampilkan data yang telah dikirim dari bagian tu (views: pengajuan-tu)
</commit_message>
<xml_diff>
--- a/public/xlsx/templat-pmb.xlsx
+++ b/public/xlsx/templat-pmb.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Pemrograman\2. Web\24. Laravel 8 (PHP Framework)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3669AC76-13B7-46F8-9520-80290A75624C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1917862D-AC50-4EC8-B85F-66C0BC82BF33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,17 +25,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>No</t>
   </si>
   <si>
-    <t>nik</t>
-  </si>
-  <si>
-    <t>nama</t>
-  </si>
-  <si>
     <t>Matematika</t>
   </si>
   <si>
@@ -64,6 +58,15 @@
   </si>
   <si>
     <t>Asal Sekolah</t>
+  </si>
+  <si>
+    <t>Nama Mapel Peminatan</t>
+  </si>
+  <si>
+    <t>Nama</t>
+  </si>
+  <si>
+    <t>NIK</t>
   </si>
 </sst>
 </file>
@@ -99,13 +102,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -390,86 +399,94 @@
   <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+      <selection sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="6.85546875" customWidth="1"/>
     <col min="4" max="4" width="12.7109375" customWidth="1"/>
     <col min="5" max="5" width="17.28515625" customWidth="1"/>
     <col min="6" max="6" width="14.7109375" customWidth="1"/>
-    <col min="8" max="8" width="8.42578125" customWidth="1"/>
-    <col min="9" max="9" width="11.28515625" customWidth="1"/>
-    <col min="10" max="10" width="9.85546875" customWidth="1"/>
-    <col min="11" max="11" width="14.42578125" customWidth="1"/>
+    <col min="7" max="7" width="17" customWidth="1"/>
+    <col min="8" max="8" width="15" customWidth="1"/>
+    <col min="9" max="9" width="15.85546875" customWidth="1"/>
+    <col min="10" max="10" width="11.5703125" customWidth="1"/>
+    <col min="11" max="11" width="12.42578125" customWidth="1"/>
+    <col min="12" max="12" width="11" customWidth="1"/>
     <col min="13" max="13" width="12.85546875" customWidth="1"/>
+    <col min="14" max="14" width="17.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="2" t="s">
+      <c r="B1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="1" t="s">
+      <c r="L1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="M1" s="2" t="s">
         <v>10</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" t="s">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="G2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G2" t="s">
-        <v>7</v>
-      </c>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="9">
-    <mergeCell ref="J1:J2"/>
+  <mergeCells count="10">
+    <mergeCell ref="D1:G1"/>
+    <mergeCell ref="H1:H2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="A1:A2"/>
     <mergeCell ref="K1:K2"/>
     <mergeCell ref="L1:L2"/>
     <mergeCell ref="M1:M2"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:H1"/>
+    <mergeCell ref="J1:J2"/>
     <mergeCell ref="I1:I2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>